<commit_message>
Adding Bank, AccNo, Date to personnel upload
</commit_message>
<xml_diff>
--- a/NNPEFWEB/wwwroot/UPLOAD/PERSONNEL.xlsx
+++ b/NNPEFWEB/wwwroot/UPLOAD/PERSONNEL.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\source\repos\NN-PEF\NNPEFWEB\wwwroot\UPLOAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\CPO_NNPEF-Main\NNPEFWEB\wwwroot\UPLOAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E6F8CC-A2E9-4CCA-AFF0-5470D579FBF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>SVC_NO</t>
   </si>
@@ -84,12 +85,27 @@
   </si>
   <si>
     <t>ilekhaize.kenneth@gmail.com</t>
+  </si>
+  <si>
+    <t>BANK</t>
+  </si>
+  <si>
+    <t>ACCOUNT_NUMBER</t>
+  </si>
+  <si>
+    <t>DATE_OF_BIRTH</t>
+  </si>
+  <si>
+    <t>DATE_OF_JOINING</t>
+  </si>
+  <si>
+    <t>Wema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,9 +144,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -411,21 +428,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,8 +467,20 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -470,8 +502,20 @@
       <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>1234567890</v>
+      </c>
+      <c r="J2" s="2">
+        <v>33824</v>
+      </c>
+      <c r="K2" s="2">
+        <v>36746</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -493,8 +537,20 @@
       <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <v>1234567890</v>
+      </c>
+      <c r="J3" s="2">
+        <v>33824</v>
+      </c>
+      <c r="K3" s="2">
+        <v>36746</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -515,13 +571,25 @@
       </c>
       <c r="G4" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4">
+        <v>1234567890</v>
+      </c>
+      <c r="J4" s="2">
+        <v>33824</v>
+      </c>
+      <c r="K4" s="2">
+        <v>36746</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>